<commit_message>
Updated phone number format to remove redundant code.
</commit_message>
<xml_diff>
--- a/whatsapp/test.xlsx
+++ b/whatsapp/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/palazzetto/dev/marketing/whatsapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59CB7B87-685E-D04F-81DD-B13719D09E65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{861F4F35-6480-8145-9E65-49C79A5470DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5460" yWindow="500" windowWidth="68800" windowHeight="26600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6560" yWindow="2400" windowWidth="68800" windowHeight="26600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="database_new" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
   <si>
     <t>id</t>
   </si>
@@ -140,19 +140,10 @@
     <t>P0353050</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Comfort Design Pte Ltd</t>
-  </si>
-  <si>
-    <t>200820272D</t>
-  </si>
-  <si>
-    <t>P0469689</t>
-  </si>
-  <si>
-    <t>CASH (Comfort)</t>
+    <t>1</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
 </sst>
 </file>
@@ -216,18 +207,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor theme="0"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -270,17 +255,17 @@
     <xf numFmtId="4" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="4" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -496,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X842"/>
+  <dimension ref="A1:X702"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -537,7 +522,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -564,7 +549,7 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="L1" s="10" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="2" t="s">
@@ -605,8 +590,8 @@
       </c>
     </row>
     <row r="2" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>2</v>
+      <c r="A2" s="11">
+        <v>6</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>27</v>
@@ -614,305 +599,258 @@
       <c r="C2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="11" t="s">
         <v>29</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="13">
-        <v>1</v>
-      </c>
-      <c r="G2" s="13" t="s">
+      <c r="F2" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="13">
+      <c r="H2" s="14">
         <v>200000</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="13">
+      <c r="L2" s="11">
         <v>83883367</v>
       </c>
       <c r="P2" s="5">
-        <v>9.9590357677602964E-2</v>
+        <f t="shared" ref="P2:P4" si="0">(Q2-S2)/S2</f>
+        <v>1.836544093808145E-2</v>
       </c>
       <c r="Q2" s="8">
+        <v>186893.99</v>
+      </c>
+      <c r="R2" s="4">
+        <v>45842</v>
+      </c>
+      <c r="S2" s="8">
         <v>183523.5</v>
       </c>
-      <c r="R2" s="4">
+      <c r="T2" s="4">
         <v>45663</v>
       </c>
-      <c r="S2" s="8">
+      <c r="U2" s="8">
         <v>180966.01</v>
       </c>
-      <c r="T2" s="14">
+      <c r="V2" s="12">
         <v>45477</v>
       </c>
-      <c r="U2" s="15">
+      <c r="W2" s="13">
         <v>166901.70000000001</v>
       </c>
-      <c r="V2" s="4">
+      <c r="X2" s="4">
         <v>45294</v>
       </c>
     </row>
     <row r="3" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="11">
+        <v>7</v>
+      </c>
       <c r="B3" s="7" t="s">
         <v>27</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="11" t="s">
         <v>29</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="13">
-        <v>1</v>
-      </c>
-      <c r="G3" s="13" t="s">
+      <c r="F3" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3" s="14">
         <v>74000</v>
       </c>
-      <c r="I3" s="13" t="s">
+      <c r="I3" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="L3" s="13">
+      <c r="L3" s="11">
         <v>83883367</v>
       </c>
       <c r="P3" s="5">
-        <v>6.0719825724751479E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.3544965689948949E-2</v>
       </c>
       <c r="Q3" s="8">
+        <v>80832.38</v>
+      </c>
+      <c r="R3" s="4">
+        <v>45842</v>
+      </c>
+      <c r="S3" s="8">
         <v>79752.14</v>
       </c>
-      <c r="R3" s="4">
+      <c r="T3" s="4">
         <v>45663</v>
       </c>
-      <c r="S3" s="8">
+      <c r="U3" s="8">
         <v>77749.67</v>
       </c>
-      <c r="T3" s="14">
+      <c r="V3" s="12">
         <v>45477</v>
       </c>
-      <c r="U3" s="15">
+      <c r="W3" s="13">
         <v>75186.81</v>
       </c>
-      <c r="V3" s="4">
+      <c r="X3" s="4">
         <v>45294</v>
       </c>
     </row>
     <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="11">
+        <v>8</v>
+      </c>
       <c r="B4" s="7" t="s">
         <v>27</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="11" t="s">
         <v>29</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="13">
-        <v>1</v>
-      </c>
-      <c r="G4" s="13" t="s">
+      <c r="F4" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H4" s="14">
         <v>60000</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="I4" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="L4" s="13">
+      <c r="L4" s="11">
         <v>83883367</v>
       </c>
       <c r="P4" s="5">
-        <v>9.816422183211683E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.8322321054990338E-2</v>
       </c>
       <c r="Q4" s="8">
+        <v>55465.97</v>
+      </c>
+      <c r="R4" s="4">
+        <v>45842</v>
+      </c>
+      <c r="S4" s="8">
         <v>54467.99</v>
       </c>
-      <c r="R4" s="4">
+      <c r="T4" s="4">
         <v>45663</v>
       </c>
-      <c r="S4" s="8">
+      <c r="U4" s="8">
         <v>53746.26</v>
       </c>
-      <c r="T4" s="14">
+      <c r="V4" s="12">
         <v>45477</v>
       </c>
-      <c r="U4" s="15">
+      <c r="W4" s="13">
         <v>49599.13</v>
       </c>
-      <c r="V4" s="4">
+      <c r="X4" s="4">
         <v>45294</v>
       </c>
     </row>
     <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="F5" s="13">
-        <v>1</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5" s="13">
-        <v>2800000</v>
-      </c>
-      <c r="I5" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="L5" s="13">
-        <v>83883367</v>
-      </c>
-      <c r="P5" s="5">
-        <v>0.13529068037725023</v>
-      </c>
-      <c r="Q5" s="8">
-        <v>2949048.85</v>
-      </c>
-      <c r="R5" s="4">
-        <v>45663</v>
-      </c>
-      <c r="S5" s="8">
-        <v>2767808.16</v>
-      </c>
-      <c r="T5" s="14">
-        <v>45477</v>
-      </c>
-      <c r="U5" s="15">
-        <v>2597615.66</v>
-      </c>
-      <c r="V5" s="4">
-        <v>45294</v>
-      </c>
+      <c r="Q5" s="6"/>
     </row>
     <row r="6" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="L6" s="13"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="8"/>
-      <c r="R6" s="11"/>
-      <c r="S6" s="9"/>
-      <c r="T6" s="4"/>
+      <c r="Q6" s="6"/>
     </row>
     <row r="7" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Q7" s="6"/>
-      <c r="T7" s="4"/>
     </row>
     <row r="8" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Q8" s="6"/>
-      <c r="T8" s="4"/>
     </row>
     <row r="9" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Q9" s="6"/>
-      <c r="T9" s="4"/>
     </row>
     <row r="10" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Q10" s="6"/>
-      <c r="T10" s="4"/>
     </row>
     <row r="11" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Q11" s="6"/>
-      <c r="T11" s="4"/>
     </row>
     <row r="12" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Q12" s="6"/>
-      <c r="T12" s="4"/>
     </row>
     <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Q13" s="6"/>
-      <c r="T13" s="4"/>
     </row>
     <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Q14" s="6"/>
-      <c r="T14" s="4"/>
     </row>
     <row r="15" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Q15" s="6"/>
-      <c r="T15" s="4"/>
     </row>
     <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Q16" s="6"/>
-      <c r="T16" s="4"/>
-    </row>
-    <row r="17" spans="9:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Q17" s="6"/>
-      <c r="T17" s="4"/>
-    </row>
-    <row r="18" spans="9:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Q18" s="6"/>
     </row>
-    <row r="19" spans="9:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Q19" s="6"/>
     </row>
-    <row r="20" spans="9:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I20" s="13" t="s">
-        <v>34</v>
-      </c>
+    <row r="20" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Q20" s="6"/>
     </row>
-    <row r="21" spans="9:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Q21" s="6"/>
     </row>
-    <row r="22" spans="9:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Q22" s="6"/>
     </row>
-    <row r="23" spans="9:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Q23" s="6"/>
     </row>
-    <row r="24" spans="9:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Q24" s="6"/>
     </row>
-    <row r="25" spans="9:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Q25" s="6"/>
     </row>
-    <row r="26" spans="9:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Q26" s="6"/>
     </row>
-    <row r="27" spans="9:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Q27" s="6"/>
     </row>
-    <row r="28" spans="9:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Q28" s="6"/>
     </row>
-    <row r="29" spans="9:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Q29" s="6"/>
     </row>
-    <row r="30" spans="9:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Q30" s="6"/>
     </row>
-    <row r="31" spans="9:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Q31" s="6"/>
     </row>
-    <row r="32" spans="9:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Q32" s="6"/>
     </row>
     <row r="33" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2924,426 +2862,6 @@
     </row>
     <row r="702" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Q702" s="6"/>
-    </row>
-    <row r="703" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q703" s="6"/>
-    </row>
-    <row r="704" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q704" s="6"/>
-    </row>
-    <row r="705" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q705" s="6"/>
-    </row>
-    <row r="706" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q706" s="6"/>
-    </row>
-    <row r="707" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q707" s="6"/>
-    </row>
-    <row r="708" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q708" s="6"/>
-    </row>
-    <row r="709" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q709" s="6"/>
-    </row>
-    <row r="710" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q710" s="6"/>
-    </row>
-    <row r="711" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q711" s="6"/>
-    </row>
-    <row r="712" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q712" s="6"/>
-    </row>
-    <row r="713" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q713" s="6"/>
-    </row>
-    <row r="714" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q714" s="6"/>
-    </row>
-    <row r="715" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q715" s="6"/>
-    </row>
-    <row r="716" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q716" s="6"/>
-    </row>
-    <row r="717" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q717" s="6"/>
-    </row>
-    <row r="718" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q718" s="6"/>
-    </row>
-    <row r="719" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q719" s="6"/>
-    </row>
-    <row r="720" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q720" s="6"/>
-    </row>
-    <row r="721" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q721" s="6"/>
-    </row>
-    <row r="722" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q722" s="6"/>
-    </row>
-    <row r="723" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q723" s="6"/>
-    </row>
-    <row r="724" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q724" s="6"/>
-    </row>
-    <row r="725" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q725" s="6"/>
-    </row>
-    <row r="726" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q726" s="6"/>
-    </row>
-    <row r="727" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q727" s="6"/>
-    </row>
-    <row r="728" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q728" s="6"/>
-    </row>
-    <row r="729" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q729" s="6"/>
-    </row>
-    <row r="730" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q730" s="6"/>
-    </row>
-    <row r="731" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q731" s="6"/>
-    </row>
-    <row r="732" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q732" s="6"/>
-    </row>
-    <row r="733" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q733" s="6"/>
-    </row>
-    <row r="734" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q734" s="6"/>
-    </row>
-    <row r="735" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q735" s="6"/>
-    </row>
-    <row r="736" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q736" s="6"/>
-    </row>
-    <row r="737" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q737" s="6"/>
-    </row>
-    <row r="738" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q738" s="6"/>
-    </row>
-    <row r="739" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q739" s="6"/>
-    </row>
-    <row r="740" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q740" s="6"/>
-    </row>
-    <row r="741" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q741" s="6"/>
-    </row>
-    <row r="742" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q742" s="6"/>
-    </row>
-    <row r="743" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q743" s="6"/>
-    </row>
-    <row r="744" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q744" s="6"/>
-    </row>
-    <row r="745" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q745" s="6"/>
-    </row>
-    <row r="746" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q746" s="6"/>
-    </row>
-    <row r="747" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q747" s="6"/>
-    </row>
-    <row r="748" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q748" s="6"/>
-    </row>
-    <row r="749" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q749" s="6"/>
-    </row>
-    <row r="750" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q750" s="6"/>
-    </row>
-    <row r="751" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q751" s="6"/>
-    </row>
-    <row r="752" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q752" s="6"/>
-    </row>
-    <row r="753" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q753" s="6"/>
-    </row>
-    <row r="754" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q754" s="6"/>
-    </row>
-    <row r="755" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q755" s="6"/>
-    </row>
-    <row r="756" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q756" s="6"/>
-    </row>
-    <row r="757" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q757" s="6"/>
-    </row>
-    <row r="758" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q758" s="6"/>
-    </row>
-    <row r="759" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q759" s="6"/>
-    </row>
-    <row r="760" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q760" s="6"/>
-    </row>
-    <row r="761" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q761" s="6"/>
-    </row>
-    <row r="762" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q762" s="6"/>
-    </row>
-    <row r="763" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q763" s="6"/>
-    </row>
-    <row r="764" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q764" s="6"/>
-    </row>
-    <row r="765" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q765" s="6"/>
-    </row>
-    <row r="766" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q766" s="6"/>
-    </row>
-    <row r="767" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q767" s="6"/>
-    </row>
-    <row r="768" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q768" s="6"/>
-    </row>
-    <row r="769" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q769" s="6"/>
-    </row>
-    <row r="770" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q770" s="6"/>
-    </row>
-    <row r="771" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q771" s="6"/>
-    </row>
-    <row r="772" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q772" s="6"/>
-    </row>
-    <row r="773" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q773" s="6"/>
-    </row>
-    <row r="774" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q774" s="6"/>
-    </row>
-    <row r="775" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q775" s="6"/>
-    </row>
-    <row r="776" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q776" s="6"/>
-    </row>
-    <row r="777" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q777" s="6"/>
-    </row>
-    <row r="778" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q778" s="6"/>
-    </row>
-    <row r="779" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q779" s="6"/>
-    </row>
-    <row r="780" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q780" s="6"/>
-    </row>
-    <row r="781" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q781" s="6"/>
-    </row>
-    <row r="782" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q782" s="6"/>
-    </row>
-    <row r="783" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q783" s="6"/>
-    </row>
-    <row r="784" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q784" s="6"/>
-    </row>
-    <row r="785" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q785" s="6"/>
-    </row>
-    <row r="786" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q786" s="6"/>
-    </row>
-    <row r="787" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q787" s="6"/>
-    </row>
-    <row r="788" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q788" s="6"/>
-    </row>
-    <row r="789" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q789" s="6"/>
-    </row>
-    <row r="790" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q790" s="6"/>
-    </row>
-    <row r="791" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q791" s="6"/>
-    </row>
-    <row r="792" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q792" s="6"/>
-    </row>
-    <row r="793" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q793" s="6"/>
-    </row>
-    <row r="794" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q794" s="6"/>
-    </row>
-    <row r="795" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q795" s="6"/>
-    </row>
-    <row r="796" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q796" s="6"/>
-    </row>
-    <row r="797" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q797" s="6"/>
-    </row>
-    <row r="798" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q798" s="6"/>
-    </row>
-    <row r="799" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q799" s="6"/>
-    </row>
-    <row r="800" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q800" s="6"/>
-    </row>
-    <row r="801" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q801" s="6"/>
-    </row>
-    <row r="802" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q802" s="6"/>
-    </row>
-    <row r="803" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q803" s="6"/>
-    </row>
-    <row r="804" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q804" s="6"/>
-    </row>
-    <row r="805" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q805" s="6"/>
-    </row>
-    <row r="806" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q806" s="6"/>
-    </row>
-    <row r="807" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q807" s="6"/>
-    </row>
-    <row r="808" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q808" s="6"/>
-    </row>
-    <row r="809" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q809" s="6"/>
-    </row>
-    <row r="810" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q810" s="6"/>
-    </row>
-    <row r="811" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q811" s="6"/>
-    </row>
-    <row r="812" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q812" s="6"/>
-    </row>
-    <row r="813" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q813" s="6"/>
-    </row>
-    <row r="814" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q814" s="6"/>
-    </row>
-    <row r="815" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q815" s="6"/>
-    </row>
-    <row r="816" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q816" s="6"/>
-    </row>
-    <row r="817" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q817" s="6"/>
-    </row>
-    <row r="818" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q818" s="6"/>
-    </row>
-    <row r="819" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q819" s="6"/>
-    </row>
-    <row r="820" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q820" s="6"/>
-    </row>
-    <row r="821" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q821" s="6"/>
-    </row>
-    <row r="822" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q822" s="6"/>
-    </row>
-    <row r="823" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q823" s="6"/>
-    </row>
-    <row r="824" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q824" s="6"/>
-    </row>
-    <row r="825" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q825" s="6"/>
-    </row>
-    <row r="826" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q826" s="6"/>
-    </row>
-    <row r="827" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q827" s="6"/>
-    </row>
-    <row r="828" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q828" s="6"/>
-    </row>
-    <row r="829" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q829" s="6"/>
-    </row>
-    <row r="830" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q830" s="6"/>
-    </row>
-    <row r="831" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q831" s="6"/>
-    </row>
-    <row r="832" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q832" s="6"/>
-    </row>
-    <row r="833" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q833" s="6"/>
-    </row>
-    <row r="834" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q834" s="6"/>
-    </row>
-    <row r="835" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q835" s="6"/>
-    </row>
-    <row r="836" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q836" s="6"/>
-    </row>
-    <row r="837" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q837" s="6"/>
-    </row>
-    <row r="838" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q838" s="6"/>
-    </row>
-    <row r="839" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q839" s="6"/>
-    </row>
-    <row r="840" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q840" s="6"/>
-    </row>
-    <row r="841" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q841" s="6"/>
-    </row>
-    <row r="842" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q842" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>

</xml_diff>